<commit_message>
Fix Kop Surat Data Mahasiswa
</commit_message>
<xml_diff>
--- a/public/data_mahasiswa/Contoh_Format_Data_Mahasiswa.xlsx
+++ b/public/data_mahasiswa/Contoh_Format_Data_Mahasiswa.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\project_tugasAkhir\public\data_mahasiswa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE780609-3987-47EE-80DE-298CD308D6B1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F807A1CE-157F-48A5-B3E8-6148B8C8AD77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="28">
   <si>
     <t>NPM</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Ayu Risqi</t>
-  </si>
-  <si>
     <t>Prodi</t>
   </si>
   <si>
@@ -63,9 +60,6 @@
     <t>Islam</t>
   </si>
   <si>
-    <t>08712361124</t>
-  </si>
-  <si>
     <t>Alamat</t>
   </si>
   <si>
@@ -79,6 +73,42 @@
   </si>
   <si>
     <t>Agama</t>
+  </si>
+  <si>
+    <t>Mahasiswa</t>
+  </si>
+  <si>
+    <t>Meto</t>
+  </si>
+  <si>
+    <t>TKK</t>
+  </si>
+  <si>
+    <t>Teklis</t>
+  </si>
+  <si>
+    <t>Kereta</t>
+  </si>
+  <si>
+    <t>Kompak</t>
+  </si>
+  <si>
+    <t>Akuntansi</t>
+  </si>
+  <si>
+    <t>Adbis</t>
+  </si>
+  <si>
+    <t>Bahasa Inggris</t>
+  </si>
+  <si>
+    <t>08712361121</t>
+  </si>
+  <si>
+    <t>08712361122</t>
+  </si>
+  <si>
+    <t>08712361123</t>
   </si>
 </sst>
 </file>
@@ -421,8 +451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,6 +460,8 @@
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
     <col min="8" max="8" width="13.140625" customWidth="1"/>
     <col min="9" max="9" width="13.28515625" customWidth="1"/>
@@ -449,27 +481,27 @@
         <v>5</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>183307037</v>
+        <v>183307001</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -478,26 +510,290 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="3" t="s">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>183307002</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
         <v>12</v>
       </c>
-      <c r="J2" t="s">
-        <v>11</v>
-      </c>
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>183307003</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>183307004</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>183307005</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>183307006</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>183307007</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>183307008</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>183307009</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+      <c r="I12" s="3"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H15" s="2"/>
@@ -505,8 +801,16 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{57021638-2BF1-4801-969C-E435FC64B8F2}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{CFB24FDE-BDEB-4076-80ED-66ACF4F69374}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{881726BE-13C3-40CD-AC31-D5260541ED5C}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{4915A7E3-2A06-4CA3-A013-4E16287DA036}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{52E1019C-2E1E-4CC8-8148-A787DF72309B}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{161290EF-FE49-421F-B33C-88C0D6919E9C}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{9F82F78C-5611-4AD0-B010-8DF2AC3D73C4}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{484971B6-BD24-49B1-92E5-4EB697716158}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{72CBD524-744F-4DFA-80BC-934475ED2B17}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>